<commit_message>
varias pruebas, el 15 ok
</commit_message>
<xml_diff>
--- a/informe_modificado.xlsx
+++ b/informe_modificado.xlsx
@@ -5,22 +5,22 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Proyectos\infDef_python\informes_defender\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matias.larenti\OneDrive - neoris.com\Desktop\Git_Codigos\infDef_python\informes_defender\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62C1F3D7-A14B-47DD-ACB4-930151B12D76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCB2CCB0-DD43-4D89-8E66-7C791A1E657C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-13620" yWindow="-12690" windowWidth="13740" windowHeight="23790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="84">
   <si>
     <t>correo</t>
   </si>
@@ -130,9 +130,6 @@
     <t>[{"UserName":"melina.villarreal","DomainName":"NEORIS","Sid":"S-1-5-21-507921405-1708537768-1957994488-188513"}]</t>
   </si>
   <si>
-    <t>alejandro.cornejo</t>
-  </si>
-  <si>
     <t>CVE-2023-35855</t>
   </si>
   <si>
@@ -259,10 +256,22 @@
     <t>matias.larenti@gmail.com</t>
   </si>
   <si>
-    <t>ale.corn12345@gmail.com</t>
-  </si>
-  <si>
     <t>eduardo.XXXXXX@hotmail.com</t>
+  </si>
+  <si>
+    <t>mildred.paez@neoris.com</t>
+  </si>
+  <si>
+    <t>sebastian.manzanares@neoris.com</t>
+  </si>
+  <si>
+    <t>mildred.paez</t>
+  </si>
+  <si>
+    <t>sebastian.manzanares</t>
+  </si>
+  <si>
+    <t>matias.larenti@neoris.com</t>
   </si>
 </sst>
 </file>
@@ -638,8 +647,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30:A42"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -690,7 +699,7 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B2" t="s">
         <v>12</v>
@@ -725,7 +734,7 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B3" t="s">
         <v>12</v>
@@ -760,7 +769,7 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="B4" t="s">
         <v>12</v>
@@ -795,7 +804,7 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="B5" t="s">
         <v>12</v>
@@ -830,7 +839,7 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="B6" t="s">
         <v>12</v>
@@ -865,7 +874,7 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="B7" t="s">
         <v>12</v>
@@ -900,7 +909,7 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="B8" t="s">
         <v>12</v>
@@ -935,7 +944,7 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="B9" t="s">
         <v>12</v>
@@ -970,16 +979,16 @@
         <v>79</v>
       </c>
       <c r="B10" t="s">
+        <v>81</v>
+      </c>
+      <c r="C10" t="s">
         <v>36</v>
-      </c>
-      <c r="C10" t="s">
-        <v>37</v>
       </c>
       <c r="D10" t="s">
         <v>32</v>
       </c>
       <c r="E10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F10" t="s">
         <v>33</v>
@@ -1002,10 +1011,10 @@
         <v>79</v>
       </c>
       <c r="B11" t="s">
-        <v>36</v>
+        <v>81</v>
       </c>
       <c r="C11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D11" t="s">
         <v>32</v>
@@ -1014,19 +1023,19 @@
         <v>23</v>
       </c>
       <c r="F11" t="s">
+        <v>39</v>
+      </c>
+      <c r="G11" t="s">
         <v>40</v>
       </c>
-      <c r="G11" t="s">
+      <c r="I11" t="s">
+        <v>18</v>
+      </c>
+      <c r="J11" t="s">
+        <v>19</v>
+      </c>
+      <c r="K11" t="s">
         <v>41</v>
-      </c>
-      <c r="I11" t="s">
-        <v>18</v>
-      </c>
-      <c r="J11" t="s">
-        <v>19</v>
-      </c>
-      <c r="K11" t="s">
-        <v>42</v>
       </c>
       <c r="L11" t="s">
         <v>35</v>
@@ -1037,10 +1046,10 @@
         <v>79</v>
       </c>
       <c r="B12" t="s">
-        <v>36</v>
+        <v>81</v>
       </c>
       <c r="C12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D12" t="s">
         <v>32</v>
@@ -1049,19 +1058,19 @@
         <v>23</v>
       </c>
       <c r="F12" t="s">
+        <v>39</v>
+      </c>
+      <c r="G12" t="s">
         <v>40</v>
       </c>
-      <c r="G12" t="s">
+      <c r="I12" t="s">
+        <v>18</v>
+      </c>
+      <c r="J12" t="s">
+        <v>19</v>
+      </c>
+      <c r="K12" t="s">
         <v>41</v>
-      </c>
-      <c r="I12" t="s">
-        <v>18</v>
-      </c>
-      <c r="J12" t="s">
-        <v>19</v>
-      </c>
-      <c r="K12" t="s">
-        <v>42</v>
       </c>
       <c r="L12" t="s">
         <v>35</v>
@@ -1072,7 +1081,7 @@
         <v>79</v>
       </c>
       <c r="B13" t="s">
-        <v>36</v>
+        <v>81</v>
       </c>
       <c r="C13" t="s">
         <v>25</v>
@@ -1107,7 +1116,7 @@
         <v>79</v>
       </c>
       <c r="B14" t="s">
-        <v>36</v>
+        <v>81</v>
       </c>
       <c r="C14" t="s">
         <v>26</v>
@@ -1142,10 +1151,10 @@
         <v>79</v>
       </c>
       <c r="B15" t="s">
-        <v>36</v>
+        <v>81</v>
       </c>
       <c r="C15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D15" t="s">
         <v>32</v>
@@ -1154,19 +1163,19 @@
         <v>15</v>
       </c>
       <c r="F15" t="s">
+        <v>44</v>
+      </c>
+      <c r="G15" t="s">
         <v>45</v>
       </c>
-      <c r="G15" t="s">
+      <c r="I15" t="s">
+        <v>18</v>
+      </c>
+      <c r="J15" t="s">
+        <v>19</v>
+      </c>
+      <c r="K15" t="s">
         <v>46</v>
-      </c>
-      <c r="I15" t="s">
-        <v>18</v>
-      </c>
-      <c r="J15" t="s">
-        <v>19</v>
-      </c>
-      <c r="K15" t="s">
-        <v>47</v>
       </c>
       <c r="L15" t="s">
         <v>35</v>
@@ -1177,23 +1186,23 @@
         <v>79</v>
       </c>
       <c r="B16" t="s">
-        <v>36</v>
+        <v>81</v>
       </c>
       <c r="C16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E16" t="s">
         <v>23</v>
       </c>
       <c r="F16" t="s">
+        <v>49</v>
+      </c>
+      <c r="G16" t="s">
         <v>50</v>
       </c>
-      <c r="G16" t="s">
-        <v>51</v>
-      </c>
       <c r="I16" t="s">
         <v>18</v>
       </c>
@@ -1201,10 +1210,10 @@
         <v>19</v>
       </c>
       <c r="K16" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
@@ -1212,23 +1221,23 @@
         <v>79</v>
       </c>
       <c r="B17" t="s">
-        <v>36</v>
+        <v>81</v>
       </c>
       <c r="C17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E17" t="s">
         <v>15</v>
       </c>
       <c r="F17" t="s">
+        <v>49</v>
+      </c>
+      <c r="G17" t="s">
         <v>50</v>
       </c>
-      <c r="G17" t="s">
-        <v>51</v>
-      </c>
       <c r="I17" t="s">
         <v>18</v>
       </c>
@@ -1236,10 +1245,10 @@
         <v>19</v>
       </c>
       <c r="K17" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L17" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
@@ -1247,23 +1256,23 @@
         <v>79</v>
       </c>
       <c r="B18" t="s">
-        <v>36</v>
+        <v>81</v>
       </c>
       <c r="C18" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D18" t="s">
+        <v>48</v>
+      </c>
+      <c r="E18" t="s">
+        <v>37</v>
+      </c>
+      <c r="F18" t="s">
         <v>49</v>
       </c>
-      <c r="E18" t="s">
-        <v>38</v>
-      </c>
-      <c r="F18" t="s">
+      <c r="G18" t="s">
         <v>50</v>
       </c>
-      <c r="G18" t="s">
-        <v>51</v>
-      </c>
       <c r="I18" t="s">
         <v>18</v>
       </c>
@@ -1271,10 +1280,10 @@
         <v>19</v>
       </c>
       <c r="K18" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L18" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
@@ -1282,23 +1291,23 @@
         <v>79</v>
       </c>
       <c r="B19" t="s">
-        <v>36</v>
+        <v>81</v>
       </c>
       <c r="C19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D19" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E19" t="s">
         <v>15</v>
       </c>
       <c r="F19" t="s">
+        <v>49</v>
+      </c>
+      <c r="G19" t="s">
         <v>50</v>
       </c>
-      <c r="G19" t="s">
-        <v>51</v>
-      </c>
       <c r="I19" t="s">
         <v>18</v>
       </c>
@@ -1306,10 +1315,10 @@
         <v>19</v>
       </c>
       <c r="K19" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L19" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
@@ -1317,23 +1326,23 @@
         <v>79</v>
       </c>
       <c r="B20" t="s">
-        <v>36</v>
+        <v>81</v>
       </c>
       <c r="C20" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D20" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E20" t="s">
         <v>23</v>
       </c>
       <c r="F20" t="s">
+        <v>49</v>
+      </c>
+      <c r="G20" t="s">
         <v>50</v>
       </c>
-      <c r="G20" t="s">
-        <v>51</v>
-      </c>
       <c r="I20" t="s">
         <v>18</v>
       </c>
@@ -1341,10 +1350,10 @@
         <v>19</v>
       </c>
       <c r="K20" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L20" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
@@ -1352,23 +1361,23 @@
         <v>79</v>
       </c>
       <c r="B21" t="s">
-        <v>36</v>
+        <v>81</v>
       </c>
       <c r="C21" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D21" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E21" t="s">
         <v>23</v>
       </c>
       <c r="F21" t="s">
+        <v>49</v>
+      </c>
+      <c r="G21" t="s">
         <v>50</v>
       </c>
-      <c r="G21" t="s">
-        <v>51</v>
-      </c>
       <c r="I21" t="s">
         <v>18</v>
       </c>
@@ -1376,34 +1385,34 @@
         <v>19</v>
       </c>
       <c r="K21" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L21" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B22" t="s">
-        <v>12</v>
+        <v>81</v>
       </c>
       <c r="C22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D22" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E22" t="s">
         <v>23</v>
       </c>
       <c r="F22" t="s">
+        <v>49</v>
+      </c>
+      <c r="G22" t="s">
         <v>50</v>
       </c>
-      <c r="G22" t="s">
-        <v>51</v>
-      </c>
       <c r="I22" t="s">
         <v>18</v>
       </c>
@@ -1411,34 +1420,34 @@
         <v>19</v>
       </c>
       <c r="K22" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L22" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B23" t="s">
-        <v>12</v>
+        <v>81</v>
       </c>
       <c r="C23" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D23" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E23" t="s">
         <v>23</v>
       </c>
       <c r="F23" t="s">
+        <v>49</v>
+      </c>
+      <c r="G23" t="s">
         <v>50</v>
       </c>
-      <c r="G23" t="s">
-        <v>51</v>
-      </c>
       <c r="I23" t="s">
         <v>18</v>
       </c>
@@ -1446,34 +1455,34 @@
         <v>19</v>
       </c>
       <c r="K23" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L23" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B24" t="s">
-        <v>12</v>
+        <v>82</v>
       </c>
       <c r="C24" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D24" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E24" t="s">
         <v>15</v>
       </c>
       <c r="F24" t="s">
+        <v>49</v>
+      </c>
+      <c r="G24" t="s">
         <v>50</v>
       </c>
-      <c r="G24" t="s">
-        <v>51</v>
-      </c>
       <c r="I24" t="s">
         <v>18</v>
       </c>
@@ -1481,34 +1490,34 @@
         <v>19</v>
       </c>
       <c r="K24" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L24" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B25" t="s">
-        <v>12</v>
+        <v>82</v>
       </c>
       <c r="C25" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D25" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E25" t="s">
         <v>15</v>
       </c>
       <c r="F25" t="s">
+        <v>49</v>
+      </c>
+      <c r="G25" t="s">
         <v>50</v>
       </c>
-      <c r="G25" t="s">
-        <v>51</v>
-      </c>
       <c r="I25" t="s">
         <v>18</v>
       </c>
@@ -1516,34 +1525,34 @@
         <v>19</v>
       </c>
       <c r="K25" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L25" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B26" t="s">
-        <v>12</v>
+        <v>82</v>
       </c>
       <c r="C26" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D26" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E26" t="s">
         <v>23</v>
       </c>
       <c r="F26" t="s">
+        <v>49</v>
+      </c>
+      <c r="G26" t="s">
         <v>50</v>
       </c>
-      <c r="G26" t="s">
-        <v>51</v>
-      </c>
       <c r="I26" t="s">
         <v>18</v>
       </c>
@@ -1551,34 +1560,34 @@
         <v>19</v>
       </c>
       <c r="K26" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L26" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B27" t="s">
-        <v>12</v>
+        <v>82</v>
       </c>
       <c r="C27" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D27" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E27" t="s">
         <v>15</v>
       </c>
       <c r="F27" t="s">
+        <v>49</v>
+      </c>
+      <c r="G27" t="s">
         <v>50</v>
       </c>
-      <c r="G27" t="s">
-        <v>51</v>
-      </c>
       <c r="I27" t="s">
         <v>18</v>
       </c>
@@ -1586,34 +1595,34 @@
         <v>19</v>
       </c>
       <c r="K27" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L27" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B28" t="s">
-        <v>12</v>
+        <v>82</v>
       </c>
       <c r="C28" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D28" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E28" t="s">
         <v>15</v>
       </c>
       <c r="F28" t="s">
+        <v>49</v>
+      </c>
+      <c r="G28" t="s">
         <v>50</v>
       </c>
-      <c r="G28" t="s">
-        <v>51</v>
-      </c>
       <c r="I28" t="s">
         <v>18</v>
       </c>
@@ -1621,34 +1630,34 @@
         <v>19</v>
       </c>
       <c r="K28" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L28" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B29" t="s">
-        <v>12</v>
+        <v>82</v>
       </c>
       <c r="C29" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D29" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E29" t="s">
         <v>23</v>
       </c>
       <c r="F29" t="s">
+        <v>66</v>
+      </c>
+      <c r="G29" t="s">
         <v>67</v>
       </c>
-      <c r="G29" t="s">
-        <v>68</v>
-      </c>
       <c r="I29" t="s">
         <v>18</v>
       </c>
@@ -1656,31 +1665,34 @@
         <v>19</v>
       </c>
       <c r="K29" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L29" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>80</v>
       </c>
+      <c r="B30" t="s">
+        <v>82</v>
+      </c>
       <c r="C30" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D30" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E30" t="s">
         <v>23</v>
       </c>
       <c r="F30" t="s">
+        <v>66</v>
+      </c>
+      <c r="G30" t="s">
         <v>67</v>
       </c>
-      <c r="G30" t="s">
-        <v>68</v>
-      </c>
       <c r="I30" t="s">
         <v>18</v>
       </c>
@@ -1688,31 +1700,34 @@
         <v>19</v>
       </c>
       <c r="K30" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L30" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>80</v>
       </c>
+      <c r="B31" t="s">
+        <v>82</v>
+      </c>
       <c r="C31" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D31" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E31" t="s">
         <v>23</v>
       </c>
       <c r="F31" t="s">
+        <v>66</v>
+      </c>
+      <c r="G31" t="s">
         <v>67</v>
       </c>
-      <c r="G31" t="s">
-        <v>68</v>
-      </c>
       <c r="I31" t="s">
         <v>18</v>
       </c>
@@ -1720,31 +1735,34 @@
         <v>19</v>
       </c>
       <c r="K31" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L31" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>80</v>
       </c>
+      <c r="B32" t="s">
+        <v>82</v>
+      </c>
       <c r="C32" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D32" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E32" t="s">
         <v>23</v>
       </c>
       <c r="F32" t="s">
+        <v>66</v>
+      </c>
+      <c r="G32" t="s">
         <v>67</v>
       </c>
-      <c r="G32" t="s">
-        <v>68</v>
-      </c>
       <c r="I32" t="s">
         <v>18</v>
       </c>
@@ -1752,31 +1770,34 @@
         <v>19</v>
       </c>
       <c r="K32" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L32" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>80</v>
       </c>
+      <c r="B33" t="s">
+        <v>82</v>
+      </c>
       <c r="C33" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D33" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E33" t="s">
         <v>23</v>
       </c>
       <c r="F33" t="s">
+        <v>66</v>
+      </c>
+      <c r="G33" t="s">
         <v>67</v>
       </c>
-      <c r="G33" t="s">
-        <v>68</v>
-      </c>
       <c r="I33" t="s">
         <v>18</v>
       </c>
@@ -1784,31 +1805,34 @@
         <v>19</v>
       </c>
       <c r="K33" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L33" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>80</v>
       </c>
+      <c r="B34" t="s">
+        <v>82</v>
+      </c>
       <c r="C34" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D34" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E34" t="s">
         <v>15</v>
       </c>
       <c r="F34" t="s">
+        <v>66</v>
+      </c>
+      <c r="G34" t="s">
         <v>67</v>
       </c>
-      <c r="G34" t="s">
-        <v>68</v>
-      </c>
       <c r="I34" t="s">
         <v>18</v>
       </c>
@@ -1816,31 +1840,34 @@
         <v>19</v>
       </c>
       <c r="K34" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L34" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>80</v>
       </c>
+      <c r="B35" t="s">
+        <v>82</v>
+      </c>
       <c r="C35" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D35" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E35" t="s">
         <v>23</v>
       </c>
       <c r="F35" t="s">
+        <v>66</v>
+      </c>
+      <c r="G35" t="s">
         <v>67</v>
       </c>
-      <c r="G35" t="s">
-        <v>68</v>
-      </c>
       <c r="I35" t="s">
         <v>18</v>
       </c>
@@ -1848,31 +1875,34 @@
         <v>19</v>
       </c>
       <c r="K35" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L35" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>80</v>
       </c>
+      <c r="B36" t="s">
+        <v>82</v>
+      </c>
       <c r="C36" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D36" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E36" t="s">
         <v>15</v>
       </c>
       <c r="F36" t="s">
+        <v>66</v>
+      </c>
+      <c r="G36" t="s">
         <v>67</v>
       </c>
-      <c r="G36" t="s">
-        <v>68</v>
-      </c>
       <c r="I36" t="s">
         <v>18</v>
       </c>
@@ -1880,31 +1910,34 @@
         <v>19</v>
       </c>
       <c r="K36" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L36" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>80</v>
       </c>
+      <c r="B37" t="s">
+        <v>82</v>
+      </c>
       <c r="C37" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D37" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E37" t="s">
         <v>15</v>
       </c>
       <c r="F37" t="s">
+        <v>66</v>
+      </c>
+      <c r="G37" t="s">
         <v>67</v>
       </c>
-      <c r="G37" t="s">
-        <v>68</v>
-      </c>
       <c r="I37" t="s">
         <v>18</v>
       </c>
@@ -1912,31 +1945,34 @@
         <v>19</v>
       </c>
       <c r="K37" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L37" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>80</v>
       </c>
+      <c r="B38" t="s">
+        <v>82</v>
+      </c>
       <c r="C38" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D38" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E38" t="s">
         <v>15</v>
       </c>
       <c r="F38" t="s">
+        <v>66</v>
+      </c>
+      <c r="G38" t="s">
         <v>67</v>
       </c>
-      <c r="G38" t="s">
-        <v>68</v>
-      </c>
       <c r="I38" t="s">
         <v>18</v>
       </c>
@@ -1944,31 +1980,34 @@
         <v>19</v>
       </c>
       <c r="K38" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L38" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>80</v>
       </c>
+      <c r="B39" t="s">
+        <v>82</v>
+      </c>
       <c r="C39" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D39" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E39" t="s">
         <v>15</v>
       </c>
       <c r="F39" t="s">
+        <v>66</v>
+      </c>
+      <c r="G39" t="s">
         <v>67</v>
       </c>
-      <c r="G39" t="s">
-        <v>68</v>
-      </c>
       <c r="I39" t="s">
         <v>18</v>
       </c>
@@ -1976,31 +2015,34 @@
         <v>19</v>
       </c>
       <c r="K39" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L39" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>80</v>
       </c>
+      <c r="B40" t="s">
+        <v>82</v>
+      </c>
       <c r="C40" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D40" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E40" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F40" t="s">
+        <v>66</v>
+      </c>
+      <c r="G40" t="s">
         <v>67</v>
       </c>
-      <c r="G40" t="s">
-        <v>68</v>
-      </c>
       <c r="I40" t="s">
         <v>18</v>
       </c>
@@ -2008,31 +2050,34 @@
         <v>19</v>
       </c>
       <c r="K40" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L40" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>80</v>
       </c>
+      <c r="B41" t="s">
+        <v>82</v>
+      </c>
       <c r="C41" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D41" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E41" t="s">
         <v>23</v>
       </c>
       <c r="F41" t="s">
+        <v>66</v>
+      </c>
+      <c r="G41" t="s">
         <v>67</v>
       </c>
-      <c r="G41" t="s">
-        <v>68</v>
-      </c>
       <c r="I41" t="s">
         <v>18</v>
       </c>
@@ -2040,31 +2085,31 @@
         <v>19</v>
       </c>
       <c r="K41" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L41" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C42" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D42" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E42" t="s">
         <v>15</v>
       </c>
       <c r="F42" t="s">
+        <v>66</v>
+      </c>
+      <c r="G42" t="s">
         <v>67</v>
       </c>
-      <c r="G42" t="s">
-        <v>68</v>
-      </c>
       <c r="I42" t="s">
         <v>18</v>
       </c>
@@ -2072,22 +2117,23 @@
         <v>19</v>
       </c>
       <c r="K42" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L42" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{BF6966DB-DF0F-4AA0-89DC-82DF6CA18E53}"/>
-    <hyperlink ref="A3:A9" r:id="rId2" display="matias.larenti@gmail.com" xr:uid="{EAD98FAF-1011-4F18-82D7-1C45D0AB441D}"/>
-    <hyperlink ref="A10" r:id="rId3" xr:uid="{D888E6EB-A648-4407-81CA-DB76A71DF959}"/>
-    <hyperlink ref="A11:A21" r:id="rId4" display="ale.corn12345@gmail.com" xr:uid="{02BBF1F4-445B-498A-A1B1-BC56DF1DE69C}"/>
-    <hyperlink ref="A22" r:id="rId5" xr:uid="{851E0646-5B4D-4C52-82D5-3C40BB5F20AD}"/>
-    <hyperlink ref="A23:A29" r:id="rId6" display="matias.larenti@gmail.com" xr:uid="{99EF9301-07A5-4D6E-91CF-D7CA0855C719}"/>
-    <hyperlink ref="A30" r:id="rId7" xr:uid="{FFF8F012-F086-4CD0-BFF8-35FA56BBD4F4}"/>
-    <hyperlink ref="A31:A42" r:id="rId8" display="eduardo.XXXXXX@hotmail.com" xr:uid="{960F457B-B5A1-4218-B89A-5FEA01E6553D}"/>
+    <hyperlink ref="A10" r:id="rId2" xr:uid="{D888E6EB-A648-4407-81CA-DB76A71DF959}"/>
+    <hyperlink ref="A23:A29" r:id="rId3" display="matias.larenti@gmail.com" xr:uid="{99EF9301-07A5-4D6E-91CF-D7CA0855C719}"/>
+    <hyperlink ref="A31:A42" r:id="rId4" display="eduardo.XXXXXX@hotmail.com" xr:uid="{960F457B-B5A1-4218-B89A-5FEA01E6553D}"/>
+    <hyperlink ref="A11:A23" r:id="rId5" display="mildred.paez@neoris.com" xr:uid="{4C57AA08-239C-471A-85C4-D3148F46E639}"/>
+    <hyperlink ref="A24" r:id="rId6" xr:uid="{9E2E5420-77A2-4EB7-84AC-D9643E05911B}"/>
+    <hyperlink ref="A25:A41" r:id="rId7" display="matias.larenti@gmail.com" xr:uid="{7FF68D39-720B-4F32-8EBF-EF6AE238025C}"/>
+    <hyperlink ref="A4" r:id="rId8" xr:uid="{0859312B-8E0E-4939-84C6-1C66FAD3B9EE}"/>
+    <hyperlink ref="A5:A9" r:id="rId9" display="matias.larenti@neoris.com" xr:uid="{5931BEB8-99C1-49DE-AA9B-FE4231DA939C}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>